<commit_message>
Doc(Journal de travail)Remplissage du journal de travail
[15][done]

J'ai compléter le journal de travail
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_Bamert_Mathieu.xlsx
+++ b/Journal-de-Travail_Bamert_Mathieu.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pv23aha\Documents\GitHub\P_AppMobile_Mathieu_Bamert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30233439-98C2-4966-A86A-DC4CBA21532C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0E9F77-1B49-4E4E-9DF0-B6E68BF77D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Autre</t>
   </si>
   <si>
-    <t>Nom Prénom</t>
-  </si>
-  <si>
     <t>P_App - 335 - Passion Lecture</t>
   </si>
   <si>
@@ -137,6 +134,18 @@
   </si>
   <si>
     <t>Création d'un figma, Ajout du modèle du téléphone, débuts de la création du figma</t>
+  </si>
+  <si>
+    <t>Présence et discussion du déroulement de l'après midi</t>
+  </si>
+  <si>
+    <t>Bamert Mathieu</t>
+  </si>
+  <si>
+    <t>Remplissage du journal de travail</t>
+  </si>
+  <si>
+    <t>J'ai continué le design de mon application mobile</t>
   </si>
 </sst>
 </file>
@@ -1073,16 +1082,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2083333333333336E-2</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.125E-2</c:v>
+                  <c:v>0.10416666666666667</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -1998,7 +2007,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2034,7 +2043,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="57"/>
@@ -2042,7 +2051,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
@@ -2051,7 +2060,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 2 heurs 15 minutes</v>
+        <v>0 jours 4 heurs 30 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2059,22 +2068,22 @@
         <v>10</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="23.25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>135</v>
+        <v>270</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2093,19 +2102,19 @@
         <v>12</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2126,7 +2135,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="54"/>
     </row>
@@ -2146,7 +2155,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="55"/>
       <c r="M8" t="s">
@@ -2175,7 +2184,7 @@
         <v>21</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="56"/>
       <c r="M9" t="s">
@@ -2189,15 +2198,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="str">
+      <c r="A10" s="8">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="46"/>
+        <v>13</v>
+      </c>
+      <c r="B10" s="46">
+        <v>45744</v>
+      </c>
       <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="36"/>
+      <c r="D10" s="48">
+        <v>15</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>31</v>
+      </c>
       <c r="G10" s="55"/>
       <c r="M10" t="s">
         <v>5</v>
@@ -2210,15 +2227,23 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="str">
+      <c r="A11" s="16">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="50"/>
+        <v>13</v>
+      </c>
+      <c r="B11" s="50">
+        <v>45744</v>
+      </c>
       <c r="C11" s="51"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="36"/>
+      <c r="D11" s="52">
+        <v>15</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>33</v>
+      </c>
       <c r="G11" s="56"/>
       <c r="M11" t="s">
         <v>6</v>
@@ -2231,15 +2256,25 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="str">
+      <c r="A12" s="8">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="36"/>
+        <v>13</v>
+      </c>
+      <c r="B12" s="46">
+        <v>45744</v>
+      </c>
+      <c r="C12" s="47">
+        <v>1</v>
+      </c>
+      <c r="D12" s="48">
+        <v>45</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="G12" s="55"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -8672,7 +8707,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8680,7 +8715,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8690,7 +8725,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8698,7 +8733,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>5.2083333333333336E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8722,11 +8757,11 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="C10" s="37" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8734,7 +8769,7 @@
       </c>
       <c r="D10" s="33">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8761,7 +8796,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>9.3750000000000014E-2</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8784,17 +8819,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9017,6 +9041,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9026,17 +9061,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9053,4 +9077,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Feat(code)J'ai commencé a coder mon app
J'ai commencé le code de mon application
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_Bamert_Mathieu.xlsx
+++ b/Journal-de-Travail_Bamert_Mathieu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pv23aha\Documents\GitHub\P_AppMobile_Mathieu_Bamert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0E9F77-1B49-4E4E-9DF0-B6E68BF77D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1071710-6AA4-4C5D-8AB7-C003AD8A7031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>J'ai continué le design de mon application mobile</t>
+  </si>
+  <si>
+    <t>J'ai designer mon application sur figma</t>
+  </si>
+  <si>
+    <t>Présence et discussion du déroulement de l'après midi et des framework</t>
+  </si>
+  <si>
+    <t>J'ai commencer à développer mon application en faisant le début de la première page et la navigation</t>
+  </si>
+  <si>
+    <t>J'ai eu un problème car je n'arrivais pas a trouver un sous-dossier pour relier à une page XAML</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1088,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1085,13 +1097,13 @@
                   <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>7.2916666666666671E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.10416666666666667</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -2007,7 +2019,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2060,7 +2072,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 4 heurs 30 minutes</v>
+        <v>0 jours 6 heurs 45 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2075,15 +2087,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>150</v>
+        <v>225</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>270</v>
+        <v>405</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2287,15 +2299,23 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="str">
+      <c r="A13" s="16">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="50"/>
+        <v>14</v>
+      </c>
+      <c r="B13" s="50">
+        <v>45751</v>
+      </c>
       <c r="C13" s="51"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="36"/>
+      <c r="D13" s="52">
+        <v>15</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>36</v>
+      </c>
       <c r="G13" s="56"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -2308,15 +2328,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="str">
+      <c r="A14" s="8">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="46"/>
+        <v>14</v>
+      </c>
+      <c r="B14" s="46">
+        <v>45751</v>
+      </c>
       <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="36"/>
+      <c r="D14" s="48">
+        <v>30</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>35</v>
+      </c>
       <c r="G14" s="55"/>
       <c r="M14" t="s">
         <v>21</v>
@@ -2328,17 +2356,29 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="str">
+    <row r="15" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="56"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="50">
+        <v>45751</v>
+      </c>
+      <c r="C15" s="51">
+        <v>1</v>
+      </c>
+      <c r="D15" s="52">
+        <v>30</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="56" t="s">
+        <v>38</v>
+      </c>
       <c r="M15" t="s">
         <v>22</v>
       </c>
@@ -8667,11 +8707,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8679,7 +8719,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8725,7 +8765,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8733,7 +8773,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>7.2916666666666671E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8761,7 +8801,7 @@
       </c>
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="C10" s="37" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8769,7 +8809,7 @@
       </c>
       <c r="D10" s="33">
         <f t="shared" si="0"/>
-        <v>0.10416666666666667</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8796,7 +8836,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.1875</v>
+        <v>0.28125000000000006</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8819,6 +8859,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9041,17 +9092,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9061,6 +9101,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9077,15 +9128,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Doc(JDT)J'ai compléter mon journal de travail
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_Bamert_Mathieu.xlsx
+++ b/Journal-de-Travail_Bamert_Mathieu.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pv23aha\Documents\GitHub\P_AppMobile_Mathieu_Bamert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1071710-6AA4-4C5D-8AB7-C003AD8A7031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AE51A6-92F3-425B-9E09-BF712614030F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="31290" yWindow="1275" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>J'ai eu un problème car je n'arrivais pas a trouver un sous-dossier pour relier à une page XAML</t>
+  </si>
+  <si>
+    <t>J'ai continuer la première page en changeant l'image et le texte</t>
+  </si>
+  <si>
+    <t>On a discuter de l'après midi et fais des pendu.</t>
+  </si>
+  <si>
+    <t>J'ai fais la connexion avec des livres. Alban m'a aidé à faire cette connexion.</t>
+  </si>
+  <si>
+    <t>J'ai commencé le crud de mon applications</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1100,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17708333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1097,7 +1109,7 @@
                   <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2916666666666671E-2</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2019,7 +2031,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2072,7 +2084,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 6 heurs 45 minutes</v>
+        <v>0 jours 9 heurs 45 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2087,15 +2099,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>225</v>
+        <v>345</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>405</v>
+        <v>585</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2390,60 +2402,94 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="str">
+      <c r="A16" s="8">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="46"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="46">
+        <v>45755</v>
+      </c>
       <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="36"/>
+      <c r="D16" s="48">
+        <v>45</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>39</v>
+      </c>
       <c r="G16" s="55"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="str">
+      <c r="A17" s="16">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="50"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="50">
+        <v>45758</v>
+      </c>
       <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="36"/>
+      <c r="D17" s="52">
+        <v>15</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>40</v>
+      </c>
       <c r="G17" s="56"/>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="str">
+      <c r="A18" s="8">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="36"/>
+        <v>15</v>
+      </c>
+      <c r="B18" s="46">
+        <v>45758</v>
+      </c>
+      <c r="C18" s="47">
+        <v>1</v>
+      </c>
+      <c r="D18" s="48">
+        <v>30</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>41</v>
+      </c>
       <c r="G18" s="55"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="str">
+      <c r="A19" s="16">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="50"/>
+        <v>15</v>
+      </c>
+      <c r="B19" s="50">
+        <v>45758</v>
+      </c>
       <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="36"/>
+      <c r="D19" s="52">
+        <v>30</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>42</v>
+      </c>
       <c r="G19" s="56"/>
       <c r="O19">
         <v>55</v>
@@ -8707,11 +8753,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8719,7 +8765,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>6.25E-2</v>
+        <v>0.17708333333333334</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8765,7 +8811,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8773,7 +8819,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>7.2916666666666671E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8836,7 +8882,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.28125000000000006</v>
+        <v>0.40625</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Feat(Rajout des epub)J'ai rajouté des epub
J'ai insérer les epubs
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_Bamert_Mathieu.xlsx
+++ b/Journal-de-Travail_Bamert_Mathieu.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pv23aha\Documents\GitHub\P_AppMobile_Mathieu_Bamert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE93453-487B-448E-ACEA-60F91EA12DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057860B9-0484-4B7C-8E2F-6691E61079B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
     <t>J'ai fais le front-end de mon app</t>
   </si>
   <si>
-    <t>J'ai vais des erreur de connexion</t>
+    <t>J'ai fais des erreur de connexion</t>
   </si>
 </sst>
 </file>
@@ -2043,7 +2043,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8953,17 +8953,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9186,6 +9175,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9195,17 +9195,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9222,4 +9211,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Doc(JDT)Remplissage du journal de travail
J'ai remplis mon journal de travail
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_Bamert_Mathieu.xlsx
+++ b/Journal-de-Travail_Bamert_Mathieu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pv23aha\Documents\GitHub\P_AppMobile_Mathieu_Bamert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057860B9-0484-4B7C-8E2F-6691E61079B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D116BD-AB4B-48D1-A6D3-34B5FA7A2EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -163,9 +163,6 @@
     <t>J'ai continuer la première page en changeant l'image et le texte</t>
   </si>
   <si>
-    <t>On a discuter de l'après midi et fais des pendu.</t>
-  </si>
-  <si>
     <t>J'ai fais la connexion avec des livres. Alban m'a aidé à faire cette connexion.</t>
   </si>
   <si>
@@ -182,6 +179,15 @@
   </si>
   <si>
     <t>J'ai fais des erreur de connexion</t>
+  </si>
+  <si>
+    <t>On a discuter de l'après midi.</t>
+  </si>
+  <si>
+    <t>discussion plaignière</t>
+  </si>
+  <si>
+    <t>Implémentation du crud</t>
   </si>
 </sst>
 </file>
@@ -1112,16 +1118,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24305555555555555</c:v>
+                  <c:v>0.3125</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7361111111111112E-2</c:v>
+                  <c:v>2.4305555555555556E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10069444444444445</c:v>
+                  <c:v>0.11805555555555555</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2043,7 +2049,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="F38" sqref="F38:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2096,7 +2102,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 11 heurs 55 minutes</v>
+        <v>0 jours 14 heurs 10 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2111,15 +2117,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>415</v>
+        <v>490</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>715</v>
+        <v>850</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2452,7 +2458,7 @@
         <v>7</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G17" s="56"/>
       <c r="O17">
@@ -2477,7 +2483,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G18" s="55"/>
       <c r="O18">
@@ -2500,7 +2506,7 @@
         <v>4</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G19" s="56"/>
       <c r="O19">
@@ -2523,7 +2529,7 @@
         <v>7</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G20" s="55"/>
     </row>
@@ -2545,10 +2551,10 @@
         <v>4</v>
       </c>
       <c r="F21" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G21" s="56" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2567,7 +2573,7 @@
         <v>4</v>
       </c>
       <c r="F22" s="36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G22" s="55"/>
     </row>
@@ -2592,39 +2598,65 @@
       <c r="G23" s="56"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="str">
+      <c r="A24" s="8">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="46"/>
+        <v>19</v>
+      </c>
+      <c r="B24" s="46">
+        <v>45784</v>
+      </c>
       <c r="C24" s="47"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="36"/>
+      <c r="D24" s="48">
+        <v>25</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>47</v>
+      </c>
       <c r="G24" s="55"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="str">
+      <c r="A25" s="16">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="36"/>
+        <v>19</v>
+      </c>
+      <c r="B25" s="50">
+        <v>45784</v>
+      </c>
+      <c r="C25" s="51">
+        <v>1</v>
+      </c>
+      <c r="D25" s="52">
+        <v>40</v>
+      </c>
+      <c r="E25" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>48</v>
+      </c>
       <c r="G25" s="56"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="str">
+      <c r="A26" s="8">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="46"/>
+        <v>19</v>
+      </c>
+      <c r="B26" s="46">
+        <v>45784</v>
+      </c>
       <c r="C26" s="47"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="36"/>
+      <c r="D26" s="48">
+        <v>10</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>33</v>
+      </c>
       <c r="G26" s="55"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -8801,11 +8833,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>170</v>
+        <v>210</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8813,7 +8845,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.24305555555555555</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8841,7 +8873,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8849,7 +8881,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>1.7361111111111112E-2</v>
+        <v>2.4305555555555556E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8859,7 +8891,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8867,7 +8899,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>0.10069444444444445</v>
+        <v>0.11805555555555555</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8930,7 +8962,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.49652777777777785</v>
+        <v>0.59027777777777779</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8953,6 +8985,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9175,17 +9218,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9195,6 +9227,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9211,15 +9254,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Feat(zip)J'ai rendu mon projet à 80%
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_Bamert_Mathieu.xlsx
+++ b/Journal-de-Travail_Bamert_Mathieu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pv23aha\Documents\GitHub\P_AppMobile_Mathieu_Bamert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D116BD-AB4B-48D1-A6D3-34B5FA7A2EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D3A3E8-204B-495A-9363-EAB7C227F651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -188,6 +188,30 @@
   </si>
   <si>
     <t>Implémentation du crud</t>
+  </si>
+  <si>
+    <t>Explication de l'après-midi</t>
+  </si>
+  <si>
+    <t>Je ne sais pas comment faire un crud pour les epub</t>
+  </si>
+  <si>
+    <t>J'ai remplis mon journal de travail</t>
+  </si>
+  <si>
+    <t>Remplis du fichier des fonctionnalité et rendre le projet à 80%</t>
+  </si>
+  <si>
+    <t>J'ai commencé le mvvm</t>
+  </si>
+  <si>
+    <t>Présentation sur le machine learning et les IA</t>
+  </si>
+  <si>
+    <t>On a discuter du déroulement de l'après midi et on a fais les évaluation des 80% projets</t>
+  </si>
+  <si>
+    <t>J'ai essayerplusieurs fa4on d'implément le mvvm mais aucune n'a fonctionner</t>
   </si>
 </sst>
 </file>
@@ -1118,19 +1142,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3125</c:v>
+                  <c:v>0.43402777777777779</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4305555555555556E-2</c:v>
+                  <c:v>5.2083333333333336E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11805555555555555</c:v>
+                  <c:v>0.15625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>6.9444444444444441E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.125</c:v>
@@ -2049,7 +2073,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F38" sqref="F38:F39"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2102,7 +2126,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 14 heurs 10 minutes</v>
+        <v>0 jours 18 heurs 49 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2117,15 +2141,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>480</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>490</v>
+        <v>650</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>850</v>
+        <v>1130</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2603,7 +2627,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="46">
-        <v>45784</v>
+        <v>45786</v>
       </c>
       <c r="C24" s="47"/>
       <c r="D24" s="48">
@@ -2623,7 +2647,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="50">
-        <v>45784</v>
+        <v>45786</v>
       </c>
       <c r="C25" s="51">
         <v>1</v>
@@ -2637,7 +2661,9 @@
       <c r="F25" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="56"/>
+      <c r="G25" s="56" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
@@ -2645,7 +2671,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="46">
-        <v>45784</v>
+        <v>45786</v>
       </c>
       <c r="C26" s="47"/>
       <c r="D26" s="48">
@@ -2660,99 +2686,167 @@
       <c r="G26" s="55"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="str">
+      <c r="A27" s="16">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="50"/>
+        <v>20</v>
+      </c>
+      <c r="B27" s="50">
+        <v>45793</v>
+      </c>
       <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="36"/>
+      <c r="D27" s="52">
+        <v>25</v>
+      </c>
+      <c r="E27" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>49</v>
+      </c>
       <c r="G27" s="56"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="str">
+      <c r="A28" s="8">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="35"/>
+        <v>20</v>
+      </c>
+      <c r="B28" s="46">
+        <v>45793</v>
+      </c>
+      <c r="C28" s="47">
+        <v>1</v>
+      </c>
+      <c r="D28" s="48">
+        <v>15</v>
+      </c>
+      <c r="E28" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>53</v>
+      </c>
       <c r="G28" s="55"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="str">
+      <c r="A29" s="16">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="50"/>
+        <v>20</v>
+      </c>
+      <c r="B29" s="50">
+        <v>45793</v>
+      </c>
       <c r="C29" s="51"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="35"/>
+      <c r="D29" s="52">
+        <v>20</v>
+      </c>
+      <c r="E29" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>52</v>
+      </c>
       <c r="G29" s="56"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="str">
+      <c r="A30" s="8">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
-        <v/>
-      </c>
-      <c r="B30" s="46"/>
+        <v>20</v>
+      </c>
+      <c r="B30" s="46">
+        <v>45793</v>
+      </c>
       <c r="C30" s="47"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="36"/>
+      <c r="D30" s="48">
+        <v>10</v>
+      </c>
+      <c r="E30" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="36" t="s">
+        <v>51</v>
+      </c>
       <c r="G30" s="55"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="str">
+      <c r="A31" s="16">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B31))</f>
-        <v/>
-      </c>
-      <c r="B31" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B31" s="50">
+        <v>45800</v>
+      </c>
       <c r="C31" s="51"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="35"/>
+      <c r="D31" s="52">
+        <v>10</v>
+      </c>
+      <c r="E31" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>54</v>
+      </c>
       <c r="G31" s="56"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="str">
+      <c r="A32" s="8">
         <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B32))</f>
-        <v/>
-      </c>
-      <c r="B32" s="46"/>
+        <v>21</v>
+      </c>
+      <c r="B32" s="46">
+        <v>45800</v>
+      </c>
       <c r="C32" s="47"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="36"/>
+      <c r="D32" s="48">
+        <v>30</v>
+      </c>
+      <c r="E32" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="36" t="s">
+        <v>55</v>
+      </c>
       <c r="G32" s="55"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="str">
+      <c r="A33" s="16">
         <f>IF(ISBLANK(B33),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B33))</f>
-        <v/>
-      </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="35"/>
+        <v>21</v>
+      </c>
+      <c r="B33" s="50">
+        <v>45800</v>
+      </c>
+      <c r="C33" s="51">
+        <v>1</v>
+      </c>
+      <c r="D33" s="52">
+        <v>40</v>
+      </c>
+      <c r="E33" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>56</v>
+      </c>
       <c r="G33" s="56"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="str">
+      <c r="A34" s="8">
         <f>IF(ISBLANK(B34),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B34))</f>
-        <v/>
-      </c>
-      <c r="B34" s="46"/>
+        <v>21</v>
+      </c>
+      <c r="B34" s="46">
+        <v>45800</v>
+      </c>
       <c r="C34" s="47"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="35"/>
+      <c r="D34" s="48">
+        <v>10</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>51</v>
+      </c>
       <c r="G34" s="55"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -8833,11 +8927,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>210</v>
+        <v>265</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8845,7 +8939,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.3125</v>
+        <v>0.43402777777777779</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8873,7 +8967,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8881,7 +8975,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>2.4305555555555556E-2</v>
+        <v>5.2083333333333336E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8891,7 +8985,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8899,7 +8993,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>0.11805555555555555</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8909,7 +9003,7 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C9" s="31" t="str">
         <f>'Journal de travail'!M13</f>
@@ -8917,7 +9011,7 @@
       </c>
       <c r="D9" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -8962,7 +9056,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.59027777777777779</v>
+        <v>0.78472222222222221</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8976,15 +9070,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -8995,7 +9080,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9218,15 +9303,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9237,7 +9323,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9254,4 +9340,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>